<commit_message>
new delta list from ElliotL@uab.edu
</commit_message>
<xml_diff>
--- a/excel_files/load_next_msl.col_map.xlsx
+++ b/excel_files/load_next_msl.col_map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\client\github\ICTVonlineDbLoad\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ICTVonlineDbLoad\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>sort</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>srcSpecies</t>
-  </si>
-  <si>
-    <t>srcIstype</t>
   </si>
   <si>
     <t>empty1</t>
@@ -461,15 +458,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -477,7 +472,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -486,6 +480,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -497,13 +494,7 @@
     <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <b val="0"/>
@@ -1048,26 +1039,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AT7" sqref="AT7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="49" max="54" width="15.25" customWidth="1"/>
+    <col min="48" max="53" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1075,38 +1066,38 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>35</v>
+      <c r="P1" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>4</v>
@@ -1117,8 +1108,8 @@
       <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
+      <c r="T1" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>7</v>
@@ -1126,270 +1117,266 @@
       <c r="V1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AF1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA1" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" s="7"/>
+      <c r="W2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AC2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AL1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AN1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AO1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW1" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="AX1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="AZ1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="BA1" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="BB1" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AE2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AF2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AG2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AH2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AI2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AK2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AL2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AM2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AN2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AO2" s="7" t="s">
+      <c r="AO2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AR2" s="7" t="s">
+      <c r="AR2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AS2" s="7" t="s">
+      <c r="AS2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AT2" s="7" t="s">
+      <c r="AT2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AU2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV2" s="13"/>
-      <c r="AW2" s="12" t="str">
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="9" t="e">
         <f ca="1">CLEAN(
 CONCATENATE(
-"insert into [",MID(AW$1,4,100),"] (",
-      AX2,
+"insert into [",MID(AV$1,4,100),"] (",
+      AW2,
       "/* "",[_comments]"" */ ",
 ") values (",
-AY2,AZ2,BA2,BB2,
-CONCATENATE("/*,_comment='loaded from ",SUBSTITUTE(CELL("filename",AX1),"'","''"),"'*/"),
+AX2,AY2,AZ2,BA2,
+CONCATENATE("/*,_comment='loaded from ",SUBSTITUTE(CELL("filename",AW1),"'","''"),"'*/"),
 "
 )"
 ))</f>
-        <v>insert into [load_next_msl] ([filename],[sort],[isWrong],[proposal_abbrev],[proposal],[spreadsheet],[srcRealm],[srcSubRealm],[srcKingdom],[srcSubkingdom],[srcPhylum],[srcSubPhylum],[srcClass],[srcSubClass],[srcOrder],[srcSubOrder],[srcFamily],[srcSubFamily],[srcGenus],[srcSubgenus],[srcSpecies],[srcIstype],[empty1],[realm],[subrealm],[kingdom],[subkingdom],[phylum],[Subphylum],[class],[subclass],[order],[suborder],[family],[subfamily],[genus],[subgenus],[species],[isType],[exemplarAccessions],[exemplarName],[abbrev],[exemplarIsolate],[isComplete],[molecule],[change],[rank]/* ",[_comments]" */ ) values (/*[filename]=*/ 'filename' ,/*[sort]=*/ 'Sort' ,/*[isWrong]=*/NULL,/*[proposal_abbrev]=*/ 'Proposals' ,/*[proposal]=*/ 'Filename' ,/*[spreadsheet]=*/ 'Spreadsheet' ,/*[srcRealm]=*/ 'Realm - Current' ,/*[srcSubRealm]=*/ 'Subrealm - Current' ,/*[srcKingdom]=*/ 'Kingdom - Current' ,/*[srcSubkingdom]=*/ 'Subkingdom - Current' ,/*[srcPhylum]=*/ 'Phylum - Current' ,/*[srcSubPhylum]=*/ 'Subphylum - Current' ,/*[srcClass]=*/ 'Class - Current' ,/*[srcSubClass]=*/ 'Subclass - Current' ,/*[srcOrder]=*/ 'Order - Current' ,/*[srcSubOrder]=*/ 'Suborder - Current' ,/*[srcFamily]=*/ 'Family - Current' ,/*[srcSubFamily]=*/ 'Subfamily - Current' ,/*[srcGenus]=*/ 'Genus - Current' ,/*[srcSubgenus]=*/ 'Subgenus - Current' ,/*[srcSpecies]=*/ 'Species - Current' ,/*[srcIstype]=*/NULL,/*[empty1]=*/NULL,/*[realm]=*/ 'Realm' ,/*[subrealm]=*/ 'Subrealm' ,/*[kingdom]=*/ 'Kingdom' ,/*[subkingdom]=*/ 'Subkingdom' ,/*[phylum]=*/ 'Phylum' ,/*[Subphylum]=*/ 'Subphylum' ,/*[class]=*/ 'Class' ,/*[subclass]=*/ 'Subclass' ,/*[order]=*/ 'Order' ,/*[suborder]=*/ 'Suborder' ,/*[family]=*/ 'Family' ,/*[subfamily]=*/ 'Subfamily' ,/*[genus]=*/ 'Genus' ,/*[subgenus]=*/ 'Subgenus' ,/*[species]=*/ 'Species' ,/*[isType]=*/ 'Type species?(1/0)' ,/*[exemplarAccessions]=*/ 'Exemplar GenBank Accession Number' ,/*[exemplarName]=*/ 'Exemplar virus name' ,/*[abbrev]=*/ 'Virus name abbrevn' ,/*[exemplarIsolate]=*/ 'Exemplar isolate designation' ,/*[isComplete]=*/ 'Genome coverage' ,/*[molecule]=*/ 'Genome composition' ,/*[change]=*/ 'Change' ,/*[rank]=*/ 'Rank' /*,_comment='loaded from D:\client\github\ICTVonlineDbLoad\excel_files\[load_next_msl.col_map.xls]col_map'*/)</v>
-      </c>
-      <c r="AX2" s="12" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="AW2" s="9" t="e">
         <f>CONCATENATE(
       CONCATENATE("[",A$1,"],[",B$1,"],[",C$1,"],[",D$1,"],[",E$1,"]"),
     CONCATENATE(",[",F$1,"],[",G$1,"],[",H$1,"],[",I$1,"],[",J$1,"]"),
     CONCATENATE(",[",K$1,"],[",L$1,"],[",M$1,"],[",N$1,"],[",O$1,"]"),
     CONCATENATE(",[",P$1,"],[",Q$1,"],[",,R$1,"],[",,S$1,"],[",,T$1,"]"),
-     CONCATENATE(",[",U$1,"],[",V$1,"],[",,W$1,"],[",,X$1,"],[",,Y$1,"]"),
-    CONCATENATE(",[",Z$1,"],[",AA$1,"],[",,AB$1,"],[",,AC$1,"],[",,AD$1,"]"),
-    CONCATENATE(",[",AE$1,"],[",AF$1,"],[",,AG$1,"],[",,AH$1,"],[",,AI$1,"]"),
-    CONCATENATE(",[",AJ$1,"],[",AK$1,"],[",,AL$1,"],[",,AM$1,"],[",,AN$1,"]"),
-    CONCATENATE(",[",AO$1,"],[",AP$1,"],[",,AQ$1,"],[",,AR$1,"],[",,AS$1,"]"),
-    CONCATENATE(",[",AT$1,"],[",AU$1,"]"),
+     CONCATENATE(",[",U$1,"],[",#REF!,"],[",,V$1,"],[",,W$1,"],[",,X$1,"]"),
+    CONCATENATE(",[",Y$1,"],[",Z$1,"],[",,AA$1,"],[",,AB$1,"],[",,AC$1,"]"),
+    CONCATENATE(",[",AD$1,"],[",AE$1,"],[",,AF$1,"],[",,AG$1,"],[",,AH$1,"]"),
+    CONCATENATE(",[",AI$1,"],[",AJ$1,"],[",,AK$1,"],[",,AL$1,"],[",,AM$1,"]"),
+    CONCATENATE(",[",AN$1,"],[",AO$1,"],[",,AP$1,"],[",,AQ$1,"],[",,AR$1,"]"),
+    CONCATENATE(",[",AS$1,"],[",AT$1,"]"),
 )</f>
-        <v>[filename],[sort],[isWrong],[proposal_abbrev],[proposal],[spreadsheet],[srcRealm],[srcSubRealm],[srcKingdom],[srcSubkingdom],[srcPhylum],[srcSubPhylum],[srcClass],[srcSubClass],[srcOrder],[srcSubOrder],[srcFamily],[srcSubFamily],[srcGenus],[srcSubgenus],[srcSpecies],[srcIstype],[empty1],[realm],[subrealm],[kingdom],[subkingdom],[phylum],[Subphylum],[class],[subclass],[order],[suborder],[family],[subfamily],[genus],[subgenus],[species],[isType],[exemplarAccessions],[exemplarName],[abbrev],[exemplarIsolate],[isComplete],[molecule],[change],[rank]</v>
-      </c>
-      <c r="AY2" s="12" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="AX2" s="9" t="str">
         <f>CONCATENATE(
 CONCATENATE("/*[",A$1,"]=*/",IF(ISBLANK(A2),"NULL",CONCATENATE(" '",SUBSTITUTE(A2,"'","''"),"' ")),
 CONCATENATE(",/*[",B$1,"]=*/",IF(ISBLANK(B2),"NULL",CONCATENATE(" '",SUBSTITUTE(B2,"'","''"),"' "))),
@@ -1409,7 +1396,7 @@
 ))</f>
         <v xml:space="preserve">/*[filename]=*/ 'filename' ,/*[sort]=*/ 'Sort' ,/*[isWrong]=*/NULL,/*[proposal_abbrev]=*/ 'Proposals' ,/*[proposal]=*/ 'Filename' ,/*[spreadsheet]=*/ 'Spreadsheet' ,/*[srcRealm]=*/ 'Realm - Current' ,/*[srcSubRealm]=*/ 'Subrealm - Current' ,/*[srcKingdom]=*/ 'Kingdom - Current' ,/*[srcSubkingdom]=*/ 'Subkingdom - Current' ,/*[srcPhylum]=*/ 'Phylum - Current' ,/*[srcSubPhylum]=*/ 'Subphylum - Current' ,/*[srcClass]=*/ 'Class - Current' ,/*[srcSubClass]=*/ 'Subclass - Current' ,/*[srcOrder]=*/ 'Order - Current' </v>
       </c>
-      <c r="AZ2" s="12" t="str">
+      <c r="AY2" s="9" t="e">
         <f>CONCATENATE(
 CONCATENATE(",/*[",P$1,"]=*/",IF(ISBLANK(P2),"NULL",CONCATENATE(" '",SUBSTITUTE(P2,"'","''"),"' " ))),
 CONCATENATE(",/*[",Q$1,"]=*/",IF(ISBLANK(Q2),"NULL",CONCATENATE(" '",SUBSTITUTE(Q2,"'","''"),"' " ))),
@@ -1417,6 +1404,7 @@
 CONCATENATE(",/*[",S$1,"]=*/",IF(ISBLANK(S2),"NULL",CONCATENATE(" '",SUBSTITUTE(S2,"'","''"),"' " ))),
 CONCATENATE(",/*[",T$1,"]=*/",IF(ISBLANK(T2),"NULL",CONCATENATE(" '",SUBSTITUTE(T2,"'","''"),"' " ))),
 CONCATENATE(",/*[",U$1,"]=*/",IF(ISBLANK(U2),"NULL",CONCATENATE(" '",SUBSTITUTE(U2,"'","''"),"' " ))),
+CONCATENATE(",/*[",#REF!,"]=*/",IF(ISBLANK(#REF!),"NULL",CONCATENATE(" '",SUBSTITUTE(#REF!,"'","''"),"' " ))),
 CONCATENATE(",/*[",V$1,"]=*/",IF(ISBLANK(V2),"NULL",CONCATENATE(" '",SUBSTITUTE(V2,"'","''"),"' " ))),
 CONCATENATE(",/*[",W$1,"]=*/",IF(ISBLANK(W2),"NULL",CONCATENATE(" '",SUBSTITUTE(W2,"'","''"),"' " ))),
 CONCATENATE(",/*[",X$1,"]=*/",IF(ISBLANK(X2),"NULL",CONCATENATE(" '",SUBSTITUTE(X2,"'","''"),"' " ))),
@@ -1425,12 +1413,12 @@
 CONCATENATE(",/*[",AA$1,"]=*/",IF(ISBLANK(AA2),"NULL",CONCATENATE(" '",SUBSTITUTE(AA2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AB$1,"]=*/",IF(ISBLANK(AB2),"NULL",CONCATENATE(" '",SUBSTITUTE(AB2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AC$1,"]=*/",IF(ISBLANK(AC2),"NULL",CONCATENATE(" '",SUBSTITUTE(AC2,"'","''"),"' " ))),
+)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AZ2" s="9" t="str">
+        <f>CONCATENATE(
 CONCATENATE(",/*[",AD$1,"]=*/",IF(ISBLANK(AD2),"NULL",CONCATENATE(" '",SUBSTITUTE(AD2,"'","''"),"' " ))),
-)</f>
-        <v xml:space="preserve">,/*[srcSubOrder]=*/ 'Suborder - Current' ,/*[srcFamily]=*/ 'Family - Current' ,/*[srcSubFamily]=*/ 'Subfamily - Current' ,/*[srcGenus]=*/ 'Genus - Current' ,/*[srcSubgenus]=*/ 'Subgenus - Current' ,/*[srcSpecies]=*/ 'Species - Current' ,/*[srcIstype]=*/NULL,/*[empty1]=*/NULL,/*[realm]=*/ 'Realm' ,/*[subrealm]=*/ 'Subrealm' ,/*[kingdom]=*/ 'Kingdom' ,/*[subkingdom]=*/ 'Subkingdom' ,/*[phylum]=*/ 'Phylum' ,/*[Subphylum]=*/ 'Subphylum' ,/*[class]=*/ 'Class' </v>
-      </c>
-      <c r="BA2" s="12" t="str">
-        <f>CONCATENATE(
 CONCATENATE(",/*[",AE$1,"]=*/",IF(ISBLANK(AE2),"NULL",CONCATENATE(" '",SUBSTITUTE(AE2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AF$1,"]=*/",IF(ISBLANK(AF2),"NULL",CONCATENATE(" '",SUBSTITUTE(AF2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AG$1,"]=*/",IF(ISBLANK(AG2),"NULL",CONCATENATE(" '",SUBSTITUTE(AG2,"'","''"),"' " ))),
@@ -1445,57 +1433,56 @@
 CONCATENATE(",/*[",AP$1,"]=*/",IF(ISBLANK(AP2),"NULL",CONCATENATE(" '",SUBSTITUTE(AP2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AQ$1,"]=*/",IF(ISBLANK(AQ2),"NULL",CONCATENATE(" '",SUBSTITUTE(AQ2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AR$1,"]=*/",IF(ISBLANK(AR2),"NULL",CONCATENATE(" '",SUBSTITUTE(AR2,"'","''"),"' " ))),
-CONCATENATE(",/*[",AS$1,"]=*/",IF(ISBLANK(AS2),"NULL",CONCATENATE(" '",SUBSTITUTE(AS2,"'","''"),"' " ))),
 )</f>
         <v xml:space="preserve">,/*[subclass]=*/ 'Subclass' ,/*[order]=*/ 'Order' ,/*[suborder]=*/ 'Suborder' ,/*[family]=*/ 'Family' ,/*[subfamily]=*/ 'Subfamily' ,/*[genus]=*/ 'Genus' ,/*[subgenus]=*/ 'Subgenus' ,/*[species]=*/ 'Species' ,/*[isType]=*/ 'Type species?
 (1/0)' ,/*[exemplarAccessions]=*/ 'Exemplar GenBank Accession Number' ,/*[exemplarName]=*/ 'Exemplar 
 virus name' ,/*[abbrev]=*/ 'Virus name abbrevn' ,/*[exemplarIsolate]=*/ 'Exemplar isolate designation' ,/*[isComplete]=*/ 'Genome coverage' ,/*[molecule]=*/ 'Genome composition
 ' </v>
       </c>
-      <c r="BB2" s="12" t="str">
+      <c r="BA2" s="9" t="str">
         <f>CONCATENATE(
+CONCATENATE(",/*[",AS$1,"]=*/",IF(ISBLANK(AS2),"NULL",CONCATENATE(" '",SUBSTITUTE(AS2,"'","''"),"' " ))),
 CONCATENATE(",/*[",AT$1,"]=*/",IF(ISBLANK(AT2),"NULL",CONCATENATE(" '",SUBSTITUTE(AT2,"'","''"),"' " ))),
-CONCATENATE(",/*[",AU$1,"]=*/",IF(ISBLANK(AU2),"NULL",CONCATENATE(" '",SUBSTITUTE(AU2,"'","''"),"' " ))),
 )</f>
         <v xml:space="preserve">,/*[change]=*/ 'Change' ,/*[rank]=*/ 'Rank' </v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="str">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="str">
         <f ca="1">MID(CELL("filename",$A$2),FIND("[",CELL("filename",$A$2))+1,FIND("]", CELL("filename",$A$2))-FIND("[",CELL("filename",$A$2))-1)</f>
-        <v>load_next_msl.col_map.xls</v>
-      </c>
-      <c r="AV3" s="13"/>
-      <c r="AW3" s="12" t="str">
+        <v>load_next_msl.col_map.xlsx</v>
+      </c>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="9" t="e">
         <f ca="1">CLEAN(
 CONCATENATE(
-"insert into [",MID(AW$1,4,100),"] (",
-      AX3,
+"insert into [",MID(AV$1,4,100),"] (",
+      AW3,
       "/* "",[_comments]"" */ ",
 ") values (",
-AY3,AZ3,BA3,BB3,
-CONCATENATE("/*,_comment='loaded from ",SUBSTITUTE(CELL("filename",AX2),"'","''"),"'*/"),
+AX3,AY3,AZ3,BA3,
+CONCATENATE("/*,_comment='loaded from ",SUBSTITUTE(CELL("filename",AW2),"'","''"),"'*/"),
 "
 )"
 ))</f>
-        <v>insert into [load_next_msl] ([filename],[sort],[isWrong],[proposal_abbrev],[proposal],[spreadsheet],[srcRealm],[srcSubRealm],[srcKingdom],[srcSubkingdom],[srcPhylum],[srcSubPhylum],[srcClass],[srcSubClass],[srcOrder],[srcSubOrder],[srcFamily],[srcSubFamily],[srcGenus],[srcSubgenus],[srcSpecies],[srcIstype],[empty1],[realm],[subrealm],[kingdom],[subkingdom],[phylum],[Subphylum],[class],[subclass],[order],[suborder],[family],[subfamily],[genus],[subgenus],[species],[isType],[exemplarAccessions],[exemplarName],[abbrev],[exemplarIsolate],[isComplete],[molecule],[change],[rank]/* ",[_comments]" */ ) values (/*[filename]=*/ 'load_next_msl.col_map.xls' ,/*[sort]=*/NULL,/*[isWrong]=*/NULL,/*[proposal_abbrev]=*/NULL,/*[proposal]=*/NULL,/*[spreadsheet]=*/NULL,/*[srcRealm]=*/NULL,/*[srcSubRealm]=*/NULL,/*[srcKingdom]=*/NULL,/*[srcSubkingdom]=*/NULL,/*[srcPhylum]=*/NULL,/*[srcSubPhylum]=*/NULL,/*[srcClass]=*/NULL,/*[srcSubClass]=*/NULL,/*[srcOrder]=*/NULL,/*[srcSubOrder]=*/NULL,/*[srcFamily]=*/NULL,/*[srcSubFamily]=*/NULL,/*[srcGenus]=*/NULL,/*[srcSubgenus]=*/NULL,/*[srcSpecies]=*/NULL,/*[srcIstype]=*/NULL,/*[empty1]=*/NULL,/*[realm]=*/NULL,/*[subrealm]=*/NULL,/*[kingdom]=*/NULL,/*[subkingdom]=*/NULL,/*[phylum]=*/NULL,/*[Subphylum]=*/NULL,/*[class]=*/NULL,/*[subclass]=*/NULL,/*[order]=*/NULL,/*[suborder]=*/NULL,/*[family]=*/NULL,/*[subfamily]=*/NULL,/*[genus]=*/NULL,/*[subgenus]=*/NULL,/*[species]=*/NULL,/*[isType]=*/NULL,/*[exemplarAccessions]=*/NULL,/*[exemplarName]=*/NULL,/*[abbrev]=*/NULL,/*[exemplarIsolate]=*/NULL,/*[isComplete]=*/NULL,/*[molecule]=*/NULL,/*[change]=*/NULL,/*[rank]=*/NULL/*,_comment='loaded from D:\client\github\ICTVonlineDbLoad\excel_files\[load_next_msl.col_map.xls]col_map'*/)</v>
-      </c>
-      <c r="AX3" s="12" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="AW3" s="9" t="e">
         <f>CONCATENATE(
       CONCATENATE("[",A$1,"],[",B$1,"],[",C$1,"],[",D$1,"],[",E$1,"]"),
     CONCATENATE(",[",F$1,"],[",G$1,"],[",H$1,"],[",I$1,"],[",J$1,"]"),
     CONCATENATE(",[",K$1,"],[",L$1,"],[",M$1,"],[",N$1,"],[",O$1,"]"),
     CONCATENATE(",[",P$1,"],[",Q$1,"],[",,R$1,"],[",,S$1,"],[",,T$1,"]"),
-     CONCATENATE(",[",U$1,"],[",V$1,"],[",,W$1,"],[",,X$1,"],[",,Y$1,"]"),
-    CONCATENATE(",[",Z$1,"],[",AA$1,"],[",,AB$1,"],[",,AC$1,"],[",,AD$1,"]"),
-    CONCATENATE(",[",AE$1,"],[",AF$1,"],[",,AG$1,"],[",,AH$1,"],[",,AI$1,"]"),
-    CONCATENATE(",[",AJ$1,"],[",AK$1,"],[",,AL$1,"],[",,AM$1,"],[",,AN$1,"]"),
-    CONCATENATE(",[",AO$1,"],[",AP$1,"],[",,AQ$1,"],[",,AR$1,"],[",,AS$1,"]"),
-    CONCATENATE(",[",AT$1,"],[",AU$1,"]"),
+     CONCATENATE(",[",U$1,"],[",#REF!,"],[",,V$1,"],[",,W$1,"],[",,X$1,"]"),
+    CONCATENATE(",[",Y$1,"],[",Z$1,"],[",,AA$1,"],[",,AB$1,"],[",,AC$1,"]"),
+    CONCATENATE(",[",AD$1,"],[",AE$1,"],[",,AF$1,"],[",,AG$1,"],[",,AH$1,"]"),
+    CONCATENATE(",[",AI$1,"],[",AJ$1,"],[",,AK$1,"],[",,AL$1,"],[",,AM$1,"]"),
+    CONCATENATE(",[",AN$1,"],[",AO$1,"],[",,AP$1,"],[",,AQ$1,"],[",,AR$1,"]"),
+    CONCATENATE(",[",AS$1,"],[",AT$1,"]"),
 )</f>
-        <v>[filename],[sort],[isWrong],[proposal_abbrev],[proposal],[spreadsheet],[srcRealm],[srcSubRealm],[srcKingdom],[srcSubkingdom],[srcPhylum],[srcSubPhylum],[srcClass],[srcSubClass],[srcOrder],[srcSubOrder],[srcFamily],[srcSubFamily],[srcGenus],[srcSubgenus],[srcSpecies],[srcIstype],[empty1],[realm],[subrealm],[kingdom],[subkingdom],[phylum],[Subphylum],[class],[subclass],[order],[suborder],[family],[subfamily],[genus],[subgenus],[species],[isType],[exemplarAccessions],[exemplarName],[abbrev],[exemplarIsolate],[isComplete],[molecule],[change],[rank]</v>
-      </c>
-      <c r="AY3" s="12" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="AX3" s="9" t="str">
         <f ca="1">CONCATENATE(
 CONCATENATE("/*[",A$1,"]=*/",IF(ISBLANK(A3),"NULL",CONCATENATE(" '",SUBSTITUTE(A3,"'","''"),"' ")),
 CONCATENATE(",/*[",B$1,"]=*/",IF(ISBLANK(B3),"NULL",CONCATENATE(" '",SUBSTITUTE(B3,"'","''"),"' "))),
@@ -1513,9 +1500,9 @@
 CONCATENATE(",/*[",N$1,"]=*/",IF(ISBLANK(N3),"NULL",CONCATENATE(" '",SUBSTITUTE(N3,"'","''"),"' "))),
 CONCATENATE(",/*[",O$1,"]=*/",IF(ISBLANK(O3),"NULL",CONCATENATE(" '",SUBSTITUTE(O3,"'","''"),"' "))),
 ))</f>
-        <v>/*[filename]=*/ 'load_next_msl.col_map.xls' ,/*[sort]=*/NULL,/*[isWrong]=*/NULL,/*[proposal_abbrev]=*/NULL,/*[proposal]=*/NULL,/*[spreadsheet]=*/NULL,/*[srcRealm]=*/NULL,/*[srcSubRealm]=*/NULL,/*[srcKingdom]=*/NULL,/*[srcSubkingdom]=*/NULL,/*[srcPhylum]=*/NULL,/*[srcSubPhylum]=*/NULL,/*[srcClass]=*/NULL,/*[srcSubClass]=*/NULL,/*[srcOrder]=*/NULL</v>
-      </c>
-      <c r="AZ3" s="12" t="str">
+        <v>/*[filename]=*/ 'load_next_msl.col_map.xlsx' ,/*[sort]=*/NULL,/*[isWrong]=*/NULL,/*[proposal_abbrev]=*/NULL,/*[proposal]=*/NULL,/*[spreadsheet]=*/NULL,/*[srcRealm]=*/NULL,/*[srcSubRealm]=*/NULL,/*[srcKingdom]=*/NULL,/*[srcSubkingdom]=*/NULL,/*[srcPhylum]=*/NULL,/*[srcSubPhylum]=*/NULL,/*[srcClass]=*/NULL,/*[srcSubClass]=*/NULL,/*[srcOrder]=*/NULL</v>
+      </c>
+      <c r="AY3" s="9" t="e">
         <f>CONCATENATE(
 CONCATENATE(",/*[",P$1,"]=*/",IF(ISBLANK(P3),"NULL",CONCATENATE(" '",SUBSTITUTE(P3,"'","''"),"' " ))),
 CONCATENATE(",/*[",Q$1,"]=*/",IF(ISBLANK(Q3),"NULL",CONCATENATE(" '",SUBSTITUTE(Q3,"'","''"),"' " ))),
@@ -1523,6 +1510,7 @@
 CONCATENATE(",/*[",S$1,"]=*/",IF(ISBLANK(S3),"NULL",CONCATENATE(" '",SUBSTITUTE(S3,"'","''"),"' " ))),
 CONCATENATE(",/*[",T$1,"]=*/",IF(ISBLANK(T3),"NULL",CONCATENATE(" '",SUBSTITUTE(T3,"'","''"),"' " ))),
 CONCATENATE(",/*[",U$1,"]=*/",IF(ISBLANK(U3),"NULL",CONCATENATE(" '",SUBSTITUTE(U3,"'","''"),"' " ))),
+CONCATENATE(",/*[",#REF!,"]=*/",IF(ISBLANK(#REF!),"NULL",CONCATENATE(" '",SUBSTITUTE(#REF!,"'","''"),"' " ))),
 CONCATENATE(",/*[",V$1,"]=*/",IF(ISBLANK(V3),"NULL",CONCATENATE(" '",SUBSTITUTE(V3,"'","''"),"' " ))),
 CONCATENATE(",/*[",W$1,"]=*/",IF(ISBLANK(W3),"NULL",CONCATENATE(" '",SUBSTITUTE(W3,"'","''"),"' " ))),
 CONCATENATE(",/*[",X$1,"]=*/",IF(ISBLANK(X3),"NULL",CONCATENATE(" '",SUBSTITUTE(X3,"'","''"),"' " ))),
@@ -1531,12 +1519,12 @@
 CONCATENATE(",/*[",AA$1,"]=*/",IF(ISBLANK(AA3),"NULL",CONCATENATE(" '",SUBSTITUTE(AA3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AB$1,"]=*/",IF(ISBLANK(AB3),"NULL",CONCATENATE(" '",SUBSTITUTE(AB3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AC$1,"]=*/",IF(ISBLANK(AC3),"NULL",CONCATENATE(" '",SUBSTITUTE(AC3,"'","''"),"' " ))),
+)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AZ3" s="9" t="str">
+        <f>CONCATENATE(
 CONCATENATE(",/*[",AD$1,"]=*/",IF(ISBLANK(AD3),"NULL",CONCATENATE(" '",SUBSTITUTE(AD3,"'","''"),"' " ))),
-)</f>
-        <v>,/*[srcSubOrder]=*/NULL,/*[srcFamily]=*/NULL,/*[srcSubFamily]=*/NULL,/*[srcGenus]=*/NULL,/*[srcSubgenus]=*/NULL,/*[srcSpecies]=*/NULL,/*[srcIstype]=*/NULL,/*[empty1]=*/NULL,/*[realm]=*/NULL,/*[subrealm]=*/NULL,/*[kingdom]=*/NULL,/*[subkingdom]=*/NULL,/*[phylum]=*/NULL,/*[Subphylum]=*/NULL,/*[class]=*/NULL</v>
-      </c>
-      <c r="BA3" s="12" t="str">
-        <f>CONCATENATE(
 CONCATENATE(",/*[",AE$1,"]=*/",IF(ISBLANK(AE3),"NULL",CONCATENATE(" '",SUBSTITUTE(AE3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AF$1,"]=*/",IF(ISBLANK(AF3),"NULL",CONCATENATE(" '",SUBSTITUTE(AF3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AG$1,"]=*/",IF(ISBLANK(AG3),"NULL",CONCATENATE(" '",SUBSTITUTE(AG3,"'","''"),"' " ))),
@@ -1551,167 +1539,161 @@
 CONCATENATE(",/*[",AP$1,"]=*/",IF(ISBLANK(AP3),"NULL",CONCATENATE(" '",SUBSTITUTE(AP3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AQ$1,"]=*/",IF(ISBLANK(AQ3),"NULL",CONCATENATE(" '",SUBSTITUTE(AQ3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AR$1,"]=*/",IF(ISBLANK(AR3),"NULL",CONCATENATE(" '",SUBSTITUTE(AR3,"'","''"),"' " ))),
-CONCATENATE(",/*[",AS$1,"]=*/",IF(ISBLANK(AS3),"NULL",CONCATENATE(" '",SUBSTITUTE(AS3,"'","''"),"' " ))),
 )</f>
         <v>,/*[subclass]=*/NULL,/*[order]=*/NULL,/*[suborder]=*/NULL,/*[family]=*/NULL,/*[subfamily]=*/NULL,/*[genus]=*/NULL,/*[subgenus]=*/NULL,/*[species]=*/NULL,/*[isType]=*/NULL,/*[exemplarAccessions]=*/NULL,/*[exemplarName]=*/NULL,/*[abbrev]=*/NULL,/*[exemplarIsolate]=*/NULL,/*[isComplete]=*/NULL,/*[molecule]=*/NULL</v>
       </c>
-      <c r="BB3" s="12" t="str">
+      <c r="BA3" s="9" t="str">
         <f>CONCATENATE(
+CONCATENATE(",/*[",AS$1,"]=*/",IF(ISBLANK(AS3),"NULL",CONCATENATE(" '",SUBSTITUTE(AS3,"'","''"),"' " ))),
 CONCATENATE(",/*[",AT$1,"]=*/",IF(ISBLANK(AT3),"NULL",CONCATENATE(" '",SUBSTITUTE(AT3,"'","''"),"' " ))),
-CONCATENATE(",/*[",AU$1,"]=*/",IF(ISBLANK(AU3),"NULL",CONCATENATE(" '",SUBSTITUTE(AU3,"'","''"),"' " ))),
 )</f>
         <v>,/*[change]=*/NULL,/*[rank]=*/NULL</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BC2:BE2">
-    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
-      <formula>BC2="Unassigned"</formula>
+  <conditionalFormatting sqref="BB2:BD2 Q1:V1 G2:V2">
+    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
+      <formula>G1="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BD2">
+    <cfRule type="cellIs" dxfId="27" priority="29" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BD2">
+    <cfRule type="cellIs" dxfId="26" priority="28" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE2">
-    <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
+      <formula>BE2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BH2">
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+      <formula>BH2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BF2">
+    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+      <formula>BF2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI2:BJ2">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+      <formula>BI2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BD2">
+    <cfRule type="cellIs" dxfId="21" priority="23" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE2">
-    <cfRule type="cellIs" dxfId="27" priority="28" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="BD2">
+    <cfRule type="cellIs" dxfId="20" priority="22" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BF2">
-    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
-      <formula>BF2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BI2">
-    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
-      <formula>BI2="Unassigned"</formula>
+  <conditionalFormatting sqref="BD2">
+    <cfRule type="cellIs" dxfId="19" priority="21" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG2">
-    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
       <formula>BG2="Unassigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BJ2:BK2">
-    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
-      <formula>BJ2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE2">
-    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="BL2">
+    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
+      <formula>BL2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BK2">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+      <formula>BK2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE1 AG1:AT1">
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+      <formula>AE1="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:AL2">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+      <formula>W2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL2">
+    <cfRule type="cellIs" dxfId="13" priority="15" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE2">
-    <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="AL2">
+    <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE2">
-    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="AM2">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+      <formula>AM2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP2">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+      <formula>AP2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN2">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+      <formula>AN2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2:AR2">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>AQ2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL2">
+    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH2">
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
-      <formula>BH2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM2">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
-      <formula>BM2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BL2">
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
-      <formula>BL2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:W1 AF1 AH1:AU1">
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
-      <formula>Q1="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:AM2">
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
-      <formula>X2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2">
-    <cfRule type="cellIs" dxfId="14" priority="15" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="AL2">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2">
-    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="AL2">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AN2">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>AN2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>AQ2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AO2">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>AO2="Unassigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR2:AS2">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
-      <formula>AR2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2">
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:W2">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>G2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP2">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>AP2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU2">
+  <conditionalFormatting sqref="AT2">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>AT2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>AS2="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>AU1="Unassigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU2:AU3">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>AU2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT2">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>AT2="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV1">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>AV1="Unassigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV2:AV3">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>AV2="Unassigned"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1723,9 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F78"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>